<commit_message>
Last bits before Windows Release.
</commit_message>
<xml_diff>
--- a/depth_chart_template.xlsx
+++ b/depth_chart_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2917DB62-E889-4BA3-8797-ACC847856C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDE9458-9D98-49E2-A002-A51C7709F0C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="depthchart_c" sheetId="5" r:id="rId1"/>
@@ -49510,7 +49510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -50234,7 +50234,7 @@
   <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+      <selection activeCell="K26" sqref="J26:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52373,7 +52373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
@@ -52984,8 +52984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG36" sqref="AG36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Last few things before merge
</commit_message>
<xml_diff>
--- a/depth_chart_template.xlsx
+++ b/depth_chart_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDE9458-9D98-49E2-A002-A51C7709F0C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE5F4DD-359A-4DEE-A3C0-CFDF06226FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="depthchart_c" sheetId="5" r:id="rId1"/>
@@ -32,9 +32,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="61">
   <si>
     <t>K VL</t>
-  </si>
-  <si>
-    <t>wRC+</t>
   </si>
   <si>
     <t>OBPplus</t>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Mov VL</t>
+  </si>
+  <si>
+    <t>wRAA</t>
   </si>
 </sst>
 </file>
@@ -5301,7 +5301,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>OBP+ and wrc+</a:t>
+              <a:t>OBP+ and wRAA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5486,7 +5486,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wRC+</c:v>
+                  <c:v>wRAA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8588,7 +8588,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>OBP+ and wrc+</a:t>
+              <a:t>OBP+ and wRAA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -8773,7 +8773,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wRC+</c:v>
+                  <c:v>wRAA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13054,7 +13054,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>OBP+ and wrc+</a:t>
+              <a:t>OBP+ and wRAA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -13239,7 +13239,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wRC+</c:v>
+                  <c:v>wRAA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -22331,7 +22331,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>OBP+ and wrc+</a:t>
+              <a:t>OBP+ and wRAA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -22516,7 +22516,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wRC+</c:v>
+                  <c:v>wRAA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -24426,7 +24426,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>OBP+ and wrc+</a:t>
+              <a:t>OBP+ and wRAA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -24611,7 +24611,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wRC+</c:v>
+                  <c:v>wRAA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -49511,7 +49511,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49551,94 +49551,94 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="N1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="W1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="X1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="17" t="s">
+      <c r="Z1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="AA1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AB1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AC1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="AD1" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="AE1" s="17" t="s">
         <v>0</v>
@@ -49827,7 +49827,7 @@
   <dimension ref="A1:BB11"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49874,100 +49874,100 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="N1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="17" t="s">
-        <v>44</v>
+      <c r="S1" s="17" t="s">
+        <v>25</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="W1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="X1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="17" t="s">
+      <c r="Z1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="AA1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AB1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AC1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AE1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AF1" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="AF1" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="AG1" s="17" t="s">
         <v>0</v>
@@ -50234,7 +50234,7 @@
   <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K26" sqref="J26:K26"/>
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50276,103 +50276,103 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="N1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="18" t="s">
-        <v>43</v>
+      <c r="R1" s="18" t="s">
+        <v>44</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="18" t="s">
-        <v>46</v>
+      <c r="T1" s="18" t="s">
+        <v>25</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="U1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="V1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="W1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="Y1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AC1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AD1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AE1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AF1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AG1" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="AG1" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="AH1" s="18" t="s">
         <v>0</v>
@@ -51038,7 +51038,7 @@
   <dimension ref="A1:AG12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="AD37" sqref="AD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51079,100 +51079,100 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="N1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="R1" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="W1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="X1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="17" t="s">
+      <c r="Z1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="AA1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AB1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AC1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AE1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AF1" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="AF1" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="AG1" s="17" t="s">
         <v>0</v>
@@ -51354,8 +51354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51396,103 +51396,103 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="N1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="19" t="s">
-        <v>53</v>
+      <c r="T1" s="19" t="s">
+        <v>25</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="AH1" s="19" t="s">
         <v>0</v>
@@ -52407,76 +52407,76 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>14</v>
-      </c>
       <c r="N1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O1" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="19" t="s">
-        <v>59</v>
-      </c>
       <c r="W1" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -52984,7 +52984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AG36" sqref="AG36"/>
     </sheetView>
   </sheetViews>
@@ -53018,76 +53018,76 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="N1" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O1" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="19" t="s">
-        <v>59</v>
-      </c>
       <c r="W1" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>